<commit_message>
Update version better Excel
Best Excel ever
</commit_message>
<xml_diff>
--- a/TestExcel.xlsx
+++ b/TestExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HenrikTingström\Documents\GitHub\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19A5D4B3-BF10-4E29-9D18-8B65AAF11C33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF0F1EF1-4D5E-49FB-B488-D33FDFAAB28D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BB4E5460-45F4-4B2E-B2DB-2EC1FD607B15}"/>
   </bookViews>
@@ -31,9 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Bla bla bla bla bla</t>
   </si>
 </sst>
 </file>
@@ -401,49 +404,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C43A5F1-1082-4D0F-B858-2541B020B341}">
-  <dimension ref="C4:C10"/>
+  <dimension ref="C4:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <f>+C5*2.5</f>
         <v>250</v>
       </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <f t="shared" ref="C7:C10" si="0">+C6*2.5</f>
         <v>625</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>1562.5</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>3906.25</v>
       </c>
     </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>9765.625</v>

</xml_diff>